<commit_message>
fix: generated name for old person (#201)
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/contact/clinic-create.xlsx
+++ b/itech-malawi/forms/contact/clinic-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
   <si>
     <t>type</t>
   </si>
@@ -207,196 +207,184 @@
     <t>Enter the name of this place</t>
   </si>
   <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>place_type_translation</t>
+  </si>
+  <si>
+    <t>jr:choice-name(${place_type},'${place_type}')</t>
+  </si>
+  <si>
+    <t>select_one generated_name</t>
+  </si>
+  <si>
+    <t>generated_name</t>
+  </si>
+  <si>
+    <t>coalesce(../../contact/name, ../name, ${custom_place_name})</t>
+  </si>
+  <si>
+    <t>generated_name_translation</t>
+  </si>
+  <si>
+    <t>jr:choice-name(${generated_name},'${generated_name}')</t>
+  </si>
+  <si>
+    <t>New Person</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>concat(${first_name}, ‘  ‘, ${surname})</t>
+  </si>
+  <si>
+    <t>person_name</t>
+  </si>
+  <si>
+    <t>../name</t>
+  </si>
+  <si>
+    <t>mpc_no</t>
+  </si>
+  <si>
+    <t>MPC Patient ID</t>
+  </si>
+  <si>
+    <t>regex(., '^[A-Za-z0-9]{1,7}$')</t>
+  </si>
+  <si>
+    <t>The Patient ID should be in P1700.. format</t>
+  </si>
+  <si>
+    <t>arv_no</t>
+  </si>
+  <si>
+    <t>ARV Number</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regex(., ‘^\+265[0-9]{9}$’) </t>
+  </si>
+  <si>
+    <t>Please enter a valid mobile number</t>
+  </si>
+  <si>
+    <t>Should start with the country code +265 followed by Nine digits</t>
+  </si>
+  <si>
+    <t>alt_phone</t>
+  </si>
+  <si>
+    <t>Alternative/Next of Kin's Mobile Number</t>
+  </si>
+  <si>
+    <t>select_one language_preference</t>
+  </si>
+  <si>
+    <t>language_preference</t>
+  </si>
+  <si>
+    <t>What is this client’s language of preference for the texts?</t>
+  </si>
+  <si>
+    <t>multiline</t>
+  </si>
+  <si>
+    <t>language_code</t>
+  </si>
+  <si>
+    <t>if(selected(${language_preference}, ’english’), ‘eng’, ‘nya’)</t>
+  </si>
+  <si>
+    <t>rapidpro</t>
+  </si>
+  <si>
+    <t>optout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>../language_preference</t>
+  </si>
+  <si>
+    <t>reminders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>adherence</t>
+  </si>
+  <si>
+    <t>visit_date</t>
+  </si>
+  <si>
+    <t>now()</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>../../../inputs/user/name</t>
+  </si>
+  <si>
+    <t>created_by_person_uuid</t>
+  </si>
+  <si>
+    <t>../../../inputs/user/contact_id</t>
+  </si>
+  <si>
+    <t>created_by_place_uuid</t>
+  </si>
+  <si>
+    <t>../../../inputs/user/facility_id</t>
+  </si>
+  <si>
     <t>clinic</t>
   </si>
   <si>
-    <t>place_type_translation</t>
-  </si>
-  <si>
-    <t>jr:choice-name(${place_type},'${place_type}')</t>
-  </si>
-  <si>
-    <t>select_one generated_name</t>
-  </si>
-  <si>
-    <t>generated_name</t>
-  </si>
-  <si>
-    <t>generated_name_translation</t>
-  </si>
-  <si>
-    <t>jr:choice-name(${generated_name},'${generated_name}')</t>
-  </si>
-  <si>
-    <t>New Person</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>patient</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>concat(${first_name}, ‘  ‘, ${surname})</t>
-  </si>
-  <si>
-    <t>person_name</t>
-  </si>
-  <si>
-    <t>../name</t>
-  </si>
-  <si>
-    <t>mpc_no</t>
-  </si>
-  <si>
-    <t>MPC Patient ID</t>
-  </si>
-  <si>
-    <t>regex(., '^[A-Za-z0-9]{1,7}$')</t>
-  </si>
-  <si>
-    <t>The Patient ID should be in P1700.. format</t>
-  </si>
-  <si>
-    <t>arv_no</t>
-  </si>
-  <si>
-    <t>ARV Number</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regex(., ‘^\+265[0-9]{9}$’) </t>
-  </si>
-  <si>
-    <t>Please enter a valid mobile number</t>
-  </si>
-  <si>
-    <t>Should start with the country code +265 followed by Nine digits</t>
-  </si>
-  <si>
-    <t>alt_phone</t>
-  </si>
-  <si>
-    <t>Alternative/Next of Kin's Mobile Number</t>
-  </si>
-  <si>
-    <t>select_one language_preference</t>
-  </si>
-  <si>
-    <t>language_preference</t>
-  </si>
-  <si>
-    <t>What is this client’s language of preference for the texts?</t>
-  </si>
-  <si>
-    <t>multiline</t>
-  </si>
-  <si>
-    <t>language_code</t>
-  </si>
-  <si>
-    <t>if(selected(${language_preference}, ’english’), ‘eng’, ‘nya’)</t>
-  </si>
-  <si>
-    <t>rapidpro</t>
-  </si>
-  <si>
-    <t>RapidPro</t>
-  </si>
-  <si>
-    <t>optout</t>
-  </si>
-  <si>
-    <t>Optout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false </t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>../language_preference</t>
-  </si>
-  <si>
-    <t>reminders</t>
-  </si>
-  <si>
-    <t>Reminders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true </t>
-  </si>
-  <si>
-    <t>adherence</t>
-  </si>
-  <si>
-    <t>Adherence</t>
-  </si>
-  <si>
-    <t>visit_date</t>
-  </si>
-  <si>
-    <t>Visit Date</t>
-  </si>
-  <si>
-    <t>now()</t>
-  </si>
-  <si>
-    <t>meta</t>
-  </si>
-  <si>
-    <t>created_by</t>
-  </si>
-  <si>
-    <t>../../../inputs/user/name</t>
-  </si>
-  <si>
-    <t>created_by_person_uuid</t>
-  </si>
-  <si>
-    <t>../../../inputs/user/contact_id</t>
-  </si>
-  <si>
-    <t>created_by_place_uuid</t>
-  </si>
-  <si>
-    <t>../../../inputs/user/facility_id</t>
-  </si>
-  <si>
     <t>select_one yes_no_generated_name</t>
   </si>
   <si>
     <t>is_name_generated</t>
   </si>
   <si>
-    <t>Would you like to name the place after the primary contact: ${person_name}?</t>
+    <t>Would you like to name the place after the primary contact: ${generated_name}?</t>
   </si>
   <si>
     <t>not(selected(${create_new_person},'none'))</t>
@@ -408,7 +396,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name_translation}, “‘ Household”)</t>
+    <t>if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name} + “’s “ +${place_type})</t>
   </si>
   <si>
     <t>external_id</t>
@@ -478,9 +466,6 @@
   </si>
   <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>Household</t>
   </si>
   <si>
     <t>${contact_name}'s Health Facility</t>
@@ -2054,7 +2039,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL69"/>
+  <dimension ref="A1:AL71"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2062,8 +2047,8 @@
   <cols>
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7344" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.5" style="1" customWidth="1"/>
     <col min="6" max="7" width="10.6719" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.3516" style="1" customWidth="1"/>
@@ -3169,7 +3154,9 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="32"/>
+      <c r="J23" t="s" s="36">
+        <v>69</v>
+      </c>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
@@ -3206,7 +3193,7 @@
         <v>48</v>
       </c>
       <c r="B24" t="s" s="31">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
@@ -3216,7 +3203,7 @@
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
       <c r="J24" t="s" s="36">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
@@ -3337,7 +3324,7 @@
         <v>38</v>
       </c>
       <c r="C27" t="s" s="32">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" t="s" s="32">
@@ -3457,7 +3444,7 @@
       <c r="Q29" s="27"/>
       <c r="R29" s="27"/>
       <c r="S29" t="s" s="32">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T29" s="27"/>
       <c r="U29" s="27"/>
@@ -3484,7 +3471,7 @@
         <v>48</v>
       </c>
       <c r="B30" t="s" s="31">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s" s="32">
         <v>22</v>
@@ -3496,7 +3483,7 @@
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
       <c r="J30" t="s" s="32">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
@@ -3532,10 +3519,10 @@
         <v>24</v>
       </c>
       <c r="B31" t="s" s="31">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s" s="32">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s" s="32">
         <v>36</v>
@@ -3580,10 +3567,10 @@
         <v>24</v>
       </c>
       <c r="B32" t="s" s="31">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s" s="32">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s" s="32">
         <v>36</v>
@@ -3640,11 +3627,11 @@
       </c>
       <c r="G33" s="27"/>
       <c r="H33" t="s" s="32">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I33" s="27"/>
       <c r="J33" t="s" s="32">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
@@ -3680,7 +3667,7 @@
         <v>48</v>
       </c>
       <c r="B34" t="s" s="31">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="34"/>
@@ -3690,7 +3677,7 @@
       <c r="H34" s="32"/>
       <c r="I34" s="27"/>
       <c r="J34" t="s" s="32">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
@@ -3726,10 +3713,10 @@
         <v>24</v>
       </c>
       <c r="B35" t="s" s="31">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s" s="32">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s" s="32">
         <v>36</v>
@@ -3738,13 +3725,13 @@
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" t="s" s="32">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I35" s="27"/>
       <c r="J35" s="34"/>
       <c r="K35" s="27"/>
       <c r="L35" t="s" s="32">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M35" s="27"/>
       <c r="N35" s="27"/>
@@ -3778,10 +3765,10 @@
         <v>24</v>
       </c>
       <c r="B36" t="s" s="31">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s" s="32">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s" s="32">
         <v>36</v>
@@ -3826,10 +3813,10 @@
         <v>24</v>
       </c>
       <c r="B37" t="s" s="31">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s" s="32">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s" s="32">
         <v>36</v>
@@ -3838,15 +3825,15 @@
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
       <c r="H37" t="s" s="39">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I37" t="s" s="40">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
       <c r="L37" t="s" s="32">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
@@ -3880,25 +3867,25 @@
         <v>24</v>
       </c>
       <c r="B38" t="s" s="31">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s" s="40">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D38" s="27"/>
       <c r="E38" s="32"/>
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" t="s" s="39">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I38" t="s" s="40">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
       <c r="L38" t="s" s="32">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
@@ -3929,20 +3916,20 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" t="s" s="30">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s" s="31">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s" s="32">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s" s="32">
         <v>36</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" t="s" s="32">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
@@ -3982,7 +3969,7 @@
         <v>48</v>
       </c>
       <c r="B40" t="s" s="31">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s" s="32">
         <v>22</v>
@@ -3994,7 +3981,7 @@
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
       <c r="J40" t="s" s="32">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K40" s="27"/>
       <c r="L40" s="27"/>
@@ -4026,24 +4013,16 @@
       <c r="AL40" s="33"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" t="s" s="30">
-        <v>20</v>
-      </c>
-      <c r="B41" t="s" s="31">
-        <v>102</v>
-      </c>
-      <c r="C41" t="s" s="32">
-        <v>103</v>
-      </c>
-      <c r="D41" s="27"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="34"/>
       <c r="E41" s="32"/>
-      <c r="F41" t="s" s="32">
-        <v>41</v>
-      </c>
+      <c r="F41" s="32"/>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
-      <c r="J41" s="34"/>
+      <c r="J41" s="32"/>
       <c r="K41" s="27"/>
       <c r="L41" s="27"/>
       <c r="M41" s="27"/>
@@ -4052,7 +4031,7 @@
       <c r="P41" s="27"/>
       <c r="Q41" s="27"/>
       <c r="R41" s="27"/>
-      <c r="S41" s="32"/>
+      <c r="S41" s="27"/>
       <c r="T41" s="27"/>
       <c r="U41" s="27"/>
       <c r="V41" s="27"/>
@@ -4075,23 +4054,23 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" t="s" s="30">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s" s="31">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s" s="32">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" t="s" s="32">
+        <v>41</v>
+      </c>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
       <c r="I42" s="27"/>
-      <c r="J42" t="s" s="32">
-        <v>106</v>
-      </c>
+      <c r="J42" s="34"/>
       <c r="K42" s="27"/>
       <c r="L42" s="27"/>
       <c r="M42" s="27"/>
@@ -4126,11 +4105,9 @@
         <v>48</v>
       </c>
       <c r="B43" t="s" s="31">
-        <v>107</v>
-      </c>
-      <c r="C43" t="s" s="32">
-        <v>108</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C43" s="32"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="32"/>
@@ -4138,7 +4115,7 @@
       <c r="H43" s="27"/>
       <c r="I43" s="27"/>
       <c r="J43" t="s" s="32">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K43" s="27"/>
       <c r="L43" s="27"/>
@@ -4174,11 +4151,9 @@
         <v>48</v>
       </c>
       <c r="B44" t="s" s="31">
-        <v>110</v>
-      </c>
-      <c r="C44" t="s" s="32">
-        <v>111</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C44" s="32"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="32"/>
@@ -4186,7 +4161,7 @@
       <c r="H44" s="27"/>
       <c r="I44" s="27"/>
       <c r="J44" t="s" s="32">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K44" s="27"/>
       <c r="L44" s="27"/>
@@ -4222,11 +4197,9 @@
         <v>48</v>
       </c>
       <c r="B45" t="s" s="31">
-        <v>113</v>
-      </c>
-      <c r="C45" t="s" s="32">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C45" s="32"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="32"/>
@@ -4234,7 +4207,7 @@
       <c r="H45" s="27"/>
       <c r="I45" s="27"/>
       <c r="J45" t="s" s="32">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K45" s="27"/>
       <c r="L45" s="27"/>
@@ -4270,11 +4243,9 @@
         <v>48</v>
       </c>
       <c r="B46" t="s" s="31">
-        <v>115</v>
-      </c>
-      <c r="C46" t="s" s="32">
-        <v>116</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C46" s="32"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="32"/>
@@ -4282,7 +4253,7 @@
       <c r="H46" s="27"/>
       <c r="I46" s="27"/>
       <c r="J46" t="s" s="32">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K46" s="27"/>
       <c r="L46" s="27"/>
@@ -4315,9 +4286,11 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" t="s" s="30">
-        <v>30</v>
-      </c>
-      <c r="B47" s="31"/>
+        <v>48</v>
+      </c>
+      <c r="B47" t="s" s="31">
+        <v>111</v>
+      </c>
       <c r="C47" s="32"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -4325,7 +4298,9 @@
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
-      <c r="J47" s="34"/>
+      <c r="J47" t="s" s="32">
+        <v>112</v>
+      </c>
       <c r="K47" s="27"/>
       <c r="L47" s="27"/>
       <c r="M47" s="27"/>
@@ -4357,23 +4332,17 @@
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" t="s" s="30">
-        <v>20</v>
-      </c>
-      <c r="B48" t="s" s="31">
-        <v>118</v>
-      </c>
-      <c r="C48" t="s" s="32">
-        <v>22</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
-      <c r="F48" t="s" s="32">
-        <v>41</v>
-      </c>
+      <c r="F48" s="32"/>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
       <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
+      <c r="J48" s="34"/>
       <c r="K48" s="27"/>
       <c r="L48" s="27"/>
       <c r="M48" s="27"/>
@@ -4382,7 +4351,7 @@
       <c r="P48" s="27"/>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
-      <c r="S48" s="27"/>
+      <c r="S48" s="32"/>
       <c r="T48" s="27"/>
       <c r="U48" s="27"/>
       <c r="V48" s="27"/>
@@ -4404,22 +4373,16 @@
       <c r="AL48" s="33"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" t="s" s="30">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s" s="31">
-        <v>119</v>
-      </c>
-      <c r="C49" s="27"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+      <c r="F49" s="32"/>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>
-      <c r="J49" t="s" s="32">
-        <v>120</v>
-      </c>
+      <c r="J49" s="34"/>
       <c r="K49" s="27"/>
       <c r="L49" s="27"/>
       <c r="M49" s="27"/>
@@ -4428,7 +4391,7 @@
       <c r="P49" s="27"/>
       <c r="Q49" s="27"/>
       <c r="R49" s="27"/>
-      <c r="S49" s="27"/>
+      <c r="S49" s="32"/>
       <c r="T49" s="27"/>
       <c r="U49" s="27"/>
       <c r="V49" s="27"/>
@@ -4451,21 +4414,23 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" t="s" s="30">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s" s="31">
-        <v>121</v>
-      </c>
-      <c r="C50" s="27"/>
+        <v>113</v>
+      </c>
+      <c r="C50" t="s" s="32">
+        <v>22</v>
+      </c>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
+      <c r="F50" t="s" s="32">
+        <v>41</v>
+      </c>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
       <c r="I50" s="27"/>
-      <c r="J50" t="s" s="32">
-        <v>122</v>
-      </c>
+      <c r="J50" s="27"/>
       <c r="K50" s="27"/>
       <c r="L50" s="27"/>
       <c r="M50" s="27"/>
@@ -4500,7 +4465,7 @@
         <v>48</v>
       </c>
       <c r="B51" t="s" s="31">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C51" s="27"/>
       <c r="D51" s="27"/>
@@ -4510,7 +4475,7 @@
       <c r="H51" s="27"/>
       <c r="I51" s="27"/>
       <c r="J51" t="s" s="32">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="K51" s="27"/>
       <c r="L51" s="27"/>
@@ -4543,9 +4508,11 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" t="s" s="30">
-        <v>30</v>
-      </c>
-      <c r="B52" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="B52" t="s" s="31">
+        <v>116</v>
+      </c>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
@@ -4553,7 +4520,9 @@
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
       <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
+      <c r="J52" t="s" s="32">
+        <v>117</v>
+      </c>
       <c r="K52" s="27"/>
       <c r="L52" s="27"/>
       <c r="M52" s="27"/>
@@ -4585,9 +4554,11 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" t="s" s="30">
-        <v>30</v>
-      </c>
-      <c r="B53" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="B53" t="s" s="31">
+        <v>118</v>
+      </c>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -4595,7 +4566,9 @@
       <c r="G53" s="27"/>
       <c r="H53" s="27"/>
       <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
+      <c r="J53" t="s" s="32">
+        <v>119</v>
+      </c>
       <c r="K53" s="27"/>
       <c r="L53" s="27"/>
       <c r="M53" s="27"/>
@@ -4626,60 +4599,56 @@
       <c r="AL53" s="33"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="23"/>
-      <c r="O54" s="24"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="26"/>
+      <c r="A54" t="s" s="30">
+        <v>30</v>
+      </c>
+      <c r="B54" s="38"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="27"/>
       <c r="R54" s="27"/>
-      <c r="S54" s="28"/>
-      <c r="T54" s="20"/>
-      <c r="U54" s="20"/>
-      <c r="V54" s="20"/>
-      <c r="W54" s="20"/>
-      <c r="X54" s="20"/>
-      <c r="Y54" s="20"/>
-      <c r="Z54" s="20"/>
-      <c r="AA54" s="20"/>
-      <c r="AB54" s="20"/>
-      <c r="AC54" s="20"/>
-      <c r="AD54" s="20"/>
-      <c r="AE54" s="20"/>
-      <c r="AF54" s="20"/>
-      <c r="AG54" s="29"/>
-      <c r="AH54" s="29"/>
-      <c r="AI54" s="29"/>
-      <c r="AJ54" s="29"/>
-      <c r="AK54" s="29"/>
-      <c r="AL54" s="29"/>
+      <c r="S54" s="27"/>
+      <c r="T54" s="27"/>
+      <c r="U54" s="27"/>
+      <c r="V54" s="27"/>
+      <c r="W54" s="27"/>
+      <c r="X54" s="27"/>
+      <c r="Y54" s="27"/>
+      <c r="Z54" s="27"/>
+      <c r="AA54" s="27"/>
+      <c r="AB54" s="27"/>
+      <c r="AC54" s="27"/>
+      <c r="AD54" s="27"/>
+      <c r="AE54" s="27"/>
+      <c r="AF54" s="27"/>
+      <c r="AG54" s="27"/>
+      <c r="AH54" s="27"/>
+      <c r="AI54" s="27"/>
+      <c r="AJ54" s="27"/>
+      <c r="AK54" s="27"/>
+      <c r="AL54" s="33"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" t="s" s="30">
-        <v>20</v>
-      </c>
-      <c r="B55" t="s" s="31">
-        <v>64</v>
-      </c>
-      <c r="C55" t="s" s="32">
-        <v>22</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B55" s="38"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
-      <c r="F55" t="s" s="32">
-        <v>32</v>
-      </c>
+      <c r="F55" s="27"/>
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
       <c r="I55" s="27"/>
@@ -4714,66 +4683,60 @@
       <c r="AL55" s="33"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" t="s" s="41">
-        <v>41</v>
-      </c>
-      <c r="B56" t="s" s="31">
-        <v>40</v>
-      </c>
-      <c r="C56" t="s" s="32">
-        <v>22</v>
-      </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="25"/>
+      <c r="Q56" s="26"/>
       <c r="R56" s="27"/>
-      <c r="S56" t="s" s="32">
-        <v>42</v>
-      </c>
-      <c r="T56" s="27"/>
-      <c r="U56" s="27"/>
-      <c r="V56" s="27"/>
-      <c r="W56" s="27"/>
-      <c r="X56" s="27"/>
-      <c r="Y56" s="27"/>
-      <c r="Z56" s="27"/>
-      <c r="AA56" s="27"/>
-      <c r="AB56" s="27"/>
-      <c r="AC56" s="27"/>
-      <c r="AD56" s="27"/>
-      <c r="AE56" s="27"/>
-      <c r="AF56" s="27"/>
-      <c r="AG56" s="27"/>
-      <c r="AH56" s="27"/>
-      <c r="AI56" s="27"/>
-      <c r="AJ56" s="27"/>
-      <c r="AK56" s="27"/>
-      <c r="AL56" s="33"/>
+      <c r="S56" s="28"/>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="20"/>
+      <c r="Y56" s="20"/>
+      <c r="Z56" s="20"/>
+      <c r="AA56" s="20"/>
+      <c r="AB56" s="20"/>
+      <c r="AC56" s="20"/>
+      <c r="AD56" s="20"/>
+      <c r="AE56" s="20"/>
+      <c r="AF56" s="20"/>
+      <c r="AG56" s="29"/>
+      <c r="AH56" s="29"/>
+      <c r="AI56" s="29"/>
+      <c r="AJ56" s="29"/>
+      <c r="AK56" s="29"/>
+      <c r="AL56" s="29"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" t="s" s="41">
-        <v>41</v>
+      <c r="A57" t="s" s="30">
+        <v>20</v>
       </c>
       <c r="B57" t="s" s="31">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s" s="32">
         <v>22</v>
       </c>
       <c r="D57" s="27"/>
       <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
+      <c r="F57" t="s" s="32">
+        <v>32</v>
+      </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
@@ -4808,24 +4771,18 @@
       <c r="AL57" s="33"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" t="s" s="30">
-        <v>125</v>
+      <c r="A58" t="s" s="41">
+        <v>41</v>
       </c>
       <c r="B58" t="s" s="31">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s" s="32">
-        <v>127</v>
-      </c>
-      <c r="D58" t="s" s="32">
-        <v>36</v>
-      </c>
-      <c r="E58" t="s" s="32">
-        <v>128</v>
-      </c>
-      <c r="F58" t="s" s="32">
-        <v>37</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
       <c r="G58" s="27"/>
       <c r="H58" s="27"/>
       <c r="I58" s="27"/>
@@ -4839,7 +4796,7 @@
       <c r="Q58" s="27"/>
       <c r="R58" s="27"/>
       <c r="S58" t="s" s="32">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="T58" s="27"/>
       <c r="U58" s="27"/>
@@ -4862,28 +4819,24 @@
       <c r="AL58" s="33"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" t="s" s="30">
-        <v>48</v>
+      <c r="A59" t="s" s="41">
+        <v>41</v>
       </c>
       <c r="B59" t="s" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="s" s="32">
-        <v>130</v>
-      </c>
-      <c r="D59" t="s" s="32">
-        <v>36</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D59" s="27"/>
       <c r="E59" s="27"/>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
       <c r="H59" s="27"/>
-      <c r="I59" s="42"/>
-      <c r="J59" t="s" s="32">
-        <v>131</v>
-      </c>
+      <c r="I59" s="27"/>
+      <c r="J59" s="27"/>
       <c r="K59" s="27"/>
-      <c r="L59" s="37"/>
+      <c r="L59" s="27"/>
       <c r="M59" s="27"/>
       <c r="N59" s="27"/>
       <c r="O59" s="27"/>
@@ -4913,17 +4866,23 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" t="s" s="30">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s" s="31">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s" s="32">
-        <v>133</v>
-      </c>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
+        <v>123</v>
+      </c>
+      <c r="D60" t="s" s="32">
+        <v>36</v>
+      </c>
+      <c r="E60" t="s" s="32">
+        <v>124</v>
+      </c>
+      <c r="F60" t="s" s="32">
+        <v>37</v>
+      </c>
       <c r="G60" s="27"/>
       <c r="H60" s="27"/>
       <c r="I60" s="27"/>
@@ -4936,7 +4895,9 @@
       <c r="P60" s="27"/>
       <c r="Q60" s="27"/>
       <c r="R60" s="27"/>
-      <c r="S60" s="27"/>
+      <c r="S60" t="s" s="32">
+        <v>125</v>
+      </c>
       <c r="T60" s="27"/>
       <c r="U60" s="27"/>
       <c r="V60" s="27"/>
@@ -4959,25 +4920,27 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" t="s" s="30">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s" s="31">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s" s="32">
-        <v>134</v>
-      </c>
-      <c r="D61" s="27"/>
+        <v>126</v>
+      </c>
+      <c r="D61" t="s" s="32">
+        <v>36</v>
+      </c>
       <c r="E61" s="27"/>
-      <c r="F61" t="s" s="32">
-        <v>99</v>
-      </c>
+      <c r="F61" s="27"/>
       <c r="G61" s="27"/>
       <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
+      <c r="I61" s="42"/>
+      <c r="J61" t="s" s="32">
+        <v>127</v>
+      </c>
       <c r="K61" s="27"/>
-      <c r="L61" s="27"/>
+      <c r="L61" s="37"/>
       <c r="M61" s="27"/>
       <c r="N61" s="27"/>
       <c r="O61" s="27"/>
@@ -5007,21 +4970,21 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" t="s" s="30">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s" s="31">
-        <v>38</v>
-      </c>
-      <c r="C62" s="27"/>
+        <v>128</v>
+      </c>
+      <c r="C62" t="s" s="32">
+        <v>129</v>
+      </c>
       <c r="D62" s="27"/>
       <c r="E62" s="27"/>
       <c r="F62" s="27"/>
       <c r="G62" s="27"/>
       <c r="H62" s="27"/>
       <c r="I62" s="27"/>
-      <c r="J62" t="s" s="32">
-        <v>135</v>
-      </c>
+      <c r="J62" s="27"/>
       <c r="K62" s="27"/>
       <c r="L62" s="27"/>
       <c r="M62" s="27"/>
@@ -5053,21 +5016,23 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" t="s" s="30">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s" s="31">
-        <v>136</v>
-      </c>
-      <c r="C63" s="27"/>
+        <v>19</v>
+      </c>
+      <c r="C63" t="s" s="32">
+        <v>130</v>
+      </c>
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
+      <c r="F63" t="s" s="32">
+        <v>100</v>
+      </c>
       <c r="G63" s="27"/>
       <c r="H63" s="27"/>
       <c r="I63" s="27"/>
-      <c r="J63" t="s" s="32">
-        <v>137</v>
-      </c>
+      <c r="J63" s="27"/>
       <c r="K63" s="27"/>
       <c r="L63" s="27"/>
       <c r="M63" s="27"/>
@@ -5099,23 +5064,21 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" t="s" s="30">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s" s="31">
-        <v>118</v>
-      </c>
-      <c r="C64" t="s" s="32">
-        <v>22</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C64" s="27"/>
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
-      <c r="F64" t="s" s="32">
-        <v>41</v>
-      </c>
+      <c r="F64" s="27"/>
       <c r="G64" s="27"/>
       <c r="H64" s="27"/>
       <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
+      <c r="J64" t="s" s="32">
+        <v>131</v>
+      </c>
       <c r="K64" s="27"/>
       <c r="L64" s="27"/>
       <c r="M64" s="27"/>
@@ -5150,7 +5113,7 @@
         <v>48</v>
       </c>
       <c r="B65" t="s" s="31">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C65" s="27"/>
       <c r="D65" s="27"/>
@@ -5160,7 +5123,7 @@
       <c r="H65" s="27"/>
       <c r="I65" s="27"/>
       <c r="J65" t="s" s="32">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="K65" s="27"/>
       <c r="L65" s="27"/>
@@ -5193,21 +5156,23 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" t="s" s="30">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s" s="31">
-        <v>121</v>
-      </c>
-      <c r="C66" s="27"/>
+        <v>113</v>
+      </c>
+      <c r="C66" t="s" s="32">
+        <v>22</v>
+      </c>
       <c r="D66" s="27"/>
       <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
+      <c r="F66" t="s" s="32">
+        <v>41</v>
+      </c>
       <c r="G66" s="27"/>
       <c r="H66" s="27"/>
       <c r="I66" s="27"/>
-      <c r="J66" t="s" s="32">
-        <v>122</v>
-      </c>
+      <c r="J66" s="27"/>
       <c r="K66" s="27"/>
       <c r="L66" s="27"/>
       <c r="M66" s="27"/>
@@ -5242,7 +5207,7 @@
         <v>48</v>
       </c>
       <c r="B67" t="s" s="31">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="27"/>
@@ -5252,7 +5217,7 @@
       <c r="H67" s="27"/>
       <c r="I67" s="27"/>
       <c r="J67" t="s" s="32">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="K67" s="27"/>
       <c r="L67" s="27"/>
@@ -5285,9 +5250,11 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" t="s" s="30">
-        <v>30</v>
-      </c>
-      <c r="B68" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="B68" t="s" s="31">
+        <v>116</v>
+      </c>
       <c r="C68" s="27"/>
       <c r="D68" s="27"/>
       <c r="E68" s="27"/>
@@ -5295,7 +5262,9 @@
       <c r="G68" s="27"/>
       <c r="H68" s="27"/>
       <c r="I68" s="27"/>
-      <c r="J68" s="27"/>
+      <c r="J68" t="s" s="32">
+        <v>117</v>
+      </c>
       <c r="K68" s="27"/>
       <c r="L68" s="27"/>
       <c r="M68" s="27"/>
@@ -5326,46 +5295,134 @@
       <c r="AL68" s="33"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" t="s" s="43">
+      <c r="A69" t="s" s="30">
+        <v>48</v>
+      </c>
+      <c r="B69" t="s" s="31">
+        <v>118</v>
+      </c>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
+      <c r="J69" t="s" s="32">
+        <v>119</v>
+      </c>
+      <c r="K69" s="27"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="27"/>
+      <c r="N69" s="27"/>
+      <c r="O69" s="27"/>
+      <c r="P69" s="27"/>
+      <c r="Q69" s="27"/>
+      <c r="R69" s="27"/>
+      <c r="S69" s="27"/>
+      <c r="T69" s="27"/>
+      <c r="U69" s="27"/>
+      <c r="V69" s="27"/>
+      <c r="W69" s="27"/>
+      <c r="X69" s="27"/>
+      <c r="Y69" s="27"/>
+      <c r="Z69" s="27"/>
+      <c r="AA69" s="27"/>
+      <c r="AB69" s="27"/>
+      <c r="AC69" s="27"/>
+      <c r="AD69" s="27"/>
+      <c r="AE69" s="27"/>
+      <c r="AF69" s="27"/>
+      <c r="AG69" s="27"/>
+      <c r="AH69" s="27"/>
+      <c r="AI69" s="27"/>
+      <c r="AJ69" s="27"/>
+      <c r="AK69" s="27"/>
+      <c r="AL69" s="33"/>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" t="s" s="30">
         <v>30</v>
       </c>
-      <c r="B69" s="44"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="45"/>
-      <c r="J69" s="45"/>
-      <c r="K69" s="45"/>
-      <c r="L69" s="45"/>
-      <c r="M69" s="45"/>
-      <c r="N69" s="45"/>
-      <c r="O69" s="45"/>
-      <c r="P69" s="45"/>
-      <c r="Q69" s="45"/>
-      <c r="R69" s="45"/>
-      <c r="S69" s="45"/>
-      <c r="T69" s="45"/>
-      <c r="U69" s="45"/>
-      <c r="V69" s="45"/>
-      <c r="W69" s="45"/>
-      <c r="X69" s="45"/>
-      <c r="Y69" s="45"/>
-      <c r="Z69" s="45"/>
-      <c r="AA69" s="45"/>
-      <c r="AB69" s="45"/>
-      <c r="AC69" s="45"/>
-      <c r="AD69" s="45"/>
-      <c r="AE69" s="45"/>
-      <c r="AF69" s="45"/>
-      <c r="AG69" s="45"/>
-      <c r="AH69" s="45"/>
-      <c r="AI69" s="45"/>
-      <c r="AJ69" s="45"/>
-      <c r="AK69" s="45"/>
-      <c r="AL69" s="46"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="27"/>
+      <c r="K70" s="27"/>
+      <c r="L70" s="27"/>
+      <c r="M70" s="27"/>
+      <c r="N70" s="27"/>
+      <c r="O70" s="27"/>
+      <c r="P70" s="27"/>
+      <c r="Q70" s="27"/>
+      <c r="R70" s="27"/>
+      <c r="S70" s="27"/>
+      <c r="T70" s="27"/>
+      <c r="U70" s="27"/>
+      <c r="V70" s="27"/>
+      <c r="W70" s="27"/>
+      <c r="X70" s="27"/>
+      <c r="Y70" s="27"/>
+      <c r="Z70" s="27"/>
+      <c r="AA70" s="27"/>
+      <c r="AB70" s="27"/>
+      <c r="AC70" s="27"/>
+      <c r="AD70" s="27"/>
+      <c r="AE70" s="27"/>
+      <c r="AF70" s="27"/>
+      <c r="AG70" s="27"/>
+      <c r="AH70" s="27"/>
+      <c r="AI70" s="27"/>
+      <c r="AJ70" s="27"/>
+      <c r="AK70" s="27"/>
+      <c r="AL70" s="33"/>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" t="s" s="43">
+        <v>30</v>
+      </c>
+      <c r="B71" s="44"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="45"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="45"/>
+      <c r="L71" s="45"/>
+      <c r="M71" s="45"/>
+      <c r="N71" s="45"/>
+      <c r="O71" s="45"/>
+      <c r="P71" s="45"/>
+      <c r="Q71" s="45"/>
+      <c r="R71" s="45"/>
+      <c r="S71" s="45"/>
+      <c r="T71" s="45"/>
+      <c r="U71" s="45"/>
+      <c r="V71" s="45"/>
+      <c r="W71" s="45"/>
+      <c r="X71" s="45"/>
+      <c r="Y71" s="45"/>
+      <c r="Z71" s="45"/>
+      <c r="AA71" s="45"/>
+      <c r="AB71" s="45"/>
+      <c r="AC71" s="45"/>
+      <c r="AD71" s="45"/>
+      <c r="AE71" s="45"/>
+      <c r="AF71" s="45"/>
+      <c r="AG71" s="45"/>
+      <c r="AH71" s="45"/>
+      <c r="AI71" s="45"/>
+      <c r="AJ71" s="45"/>
+      <c r="AK71" s="45"/>
+      <c r="AL71" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
@@ -5394,7 +5451,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="48">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s" s="48">
         <v>1</v>
@@ -5422,13 +5479,13 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="48">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s" s="48">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s" s="48">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
@@ -5450,13 +5507,13 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="48">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s" s="48">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s" s="48">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>
@@ -5481,10 +5538,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="s" s="50">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s" s="51">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
@@ -5509,10 +5566,10 @@
         <v>38</v>
       </c>
       <c r="B5" t="s" s="50">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s" s="51">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
@@ -5537,10 +5594,10 @@
         <v>38</v>
       </c>
       <c r="B6" t="s" s="50">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s" s="51">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -5562,13 +5619,13 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="48">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s" s="48">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s" s="48">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -5590,13 +5647,13 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s" s="48">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s" s="48">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s" s="48">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
@@ -5621,10 +5678,10 @@
         <v>62</v>
       </c>
       <c r="B9" t="s" s="50">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s" s="51">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -5649,10 +5706,10 @@
         <v>62</v>
       </c>
       <c r="B10" t="s" s="50">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s" s="51">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D10" s="49"/>
       <c r="E10" s="49"/>
@@ -5677,10 +5734,10 @@
         <v>62</v>
       </c>
       <c r="B11" t="s" s="50">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s" s="51">
         <v>64</v>
-      </c>
-      <c r="C11" t="s" s="51">
-        <v>155</v>
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
@@ -5705,10 +5762,10 @@
         <v>68</v>
       </c>
       <c r="B12" t="s" s="50">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s" s="51">
         <v>151</v>
-      </c>
-      <c r="C12" t="s" s="51">
-        <v>156</v>
       </c>
       <c r="D12" s="49"/>
       <c r="E12" s="49"/>
@@ -5733,10 +5790,10 @@
         <v>68</v>
       </c>
       <c r="B13" t="s" s="50">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s" s="51">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D13" s="49"/>
       <c r="E13" s="49"/>
@@ -5761,10 +5818,10 @@
         <v>68</v>
       </c>
       <c r="B14" t="s" s="50">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s" s="51">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D14" s="49"/>
       <c r="E14" s="49"/>
@@ -5786,13 +5843,13 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s" s="52">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s" s="50">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s" s="51">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D15" s="49"/>
       <c r="E15" s="49"/>
@@ -5814,13 +5871,13 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" t="s" s="53">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s" s="50">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s" s="51">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D16" s="49"/>
       <c r="E16" s="49"/>
@@ -5842,13 +5899,13 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" t="s" s="54">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s" s="55">
         <v>1</v>
       </c>
       <c r="C17" t="s" s="51">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="49"/>
@@ -5898,19 +5955,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="52">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s" s="52">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s" s="52">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D1" t="s" s="52">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s" s="52">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -5935,19 +5992,19 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="52">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="52">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s" s="52">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s" s="52">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s" s="52">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>

</xml_diff>